<commit_message>
PCB bom and rendering updates
</commit_message>
<xml_diff>
--- a/pcb/bom/bom.xlsx
+++ b/pcb/bom/bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Qty</t>
   </si>
@@ -70,43 +70,49 @@
     <t>0603 Resistor</t>
   </si>
   <si>
-    <t>ATtiny 84 MCU</t>
+    <t>ATtiny 24 MCU</t>
   </si>
   <si>
     <t>ISP Header</t>
   </si>
   <si>
-    <t>0.1µF</t>
+    <t>0.1 µF</t>
   </si>
   <si>
     <t>470 µF</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>RJ45_pyControl</t>
-  </si>
-  <si>
-    <t>10KΩ</t>
-  </si>
-  <si>
-    <t>ATtiny84-20SSU</t>
-  </si>
-  <si>
-    <t>AVR_ISP</t>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>0855135013</t>
+  </si>
+  <si>
+    <t>20KΩ</t>
+  </si>
+  <si>
+    <t>ATTINY24A-SSUR</t>
+  </si>
+  <si>
+    <t>75869-331LF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=1276-1258-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=P15094CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=160-1447-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=WM3553CT-ND</t>
   </si>
   <si>
     <t>~</t>
   </si>
   <si>
-    <t>https://www.digikey.com/products/en?keywords=P15094CT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=WM3553CT-ND</t>
-  </si>
-  <si>
-    <t>http://ww1.microchip.com/downloads/en/DeviceDoc/doc8006.pdf</t>
+    <t>https://www.digikey.com/products/en?keywords=ATTINY24A-SSURCT-ND</t>
   </si>
   <si>
     <t>https://www.digikey.com/products/en?keywords=609-5122-ND</t>
@@ -516,7 +522,7 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -550,8 +556,8 @@
       <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
-        <v>27</v>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -568,7 +574,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -585,7 +591,7 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -602,7 +608,7 @@
         <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -619,15 +625,17 @@
         <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
-    <hyperlink ref="E7" r:id="rId3"/>
-    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>